<commit_message>
Agregar formato a celdas del archivo Excel generado
</commit_message>
<xml_diff>
--- a/tp_01/factura.xlsx
+++ b/tp_01/factura.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Nro</t>
   </si>
@@ -26,7 +26,7 @@
     <t>24/11/2018</t>
   </si>
   <si>
-    <t>Razón</t>
+    <t>Razón Social</t>
   </si>
   <si>
     <t>Razon Social</t>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -46,13 +52,53 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,26 +121,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="12.96875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.70703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -102,7 +179,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -110,7 +187,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="3">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -118,47 +195,67 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="6">
         <v>8</v>
+      </c>
+      <c r="D5" t="s" s="7">
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="n" s="8">
         <v>100.5</v>
       </c>
       <c r="C6" t="n">
         <v>1.0</v>
       </c>
+      <c r="D6" t="n" s="9">
+        <v>100.5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" t="n" s="10">
         <v>100.5</v>
       </c>
       <c r="C7" t="n">
         <v>2.0</v>
       </c>
+      <c r="D7" t="n" s="11">
+        <v>201.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" t="n" s="12">
         <v>100.5</v>
       </c>
       <c r="C8" t="n">
         <v>3.0</v>
+      </c>
+      <c r="D8" t="n" s="13">
+        <v>301.5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="D9" t="n" s="15">
+        <v>603.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>